<commit_message>
feat: add design length field to cable management
- Updated the database schema to include a new column for design length in the cables table.
- Modified the CableRow and PublicCable types to accommodate the new design length property.
- Enhanced the cables routes to handle design length during create and update operations.
- Updated the validation schema to include design length with appropriate constraints.
- Adjusted the API client and forms to support design length input and display.
- Updated the ProjectDetails component to show design length in the cable dialog and list.
- Removed unused functions related to design length calculation, simplifying the codebase.
</commit_message>
<xml_diff>
--- a/Template files/Trays materials.xlsx
+++ b/Template files/Trays materials.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27722"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TOKA\source\repos\WFC\Template files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\todor.chankov\source\WFC\Template files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56908C41-C843-4493-B416-A9568EAC7FFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A4C29C-8A50-4027-93A8-0E255D1E4E83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28898" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{A602074D-93F6-4DC7-9C39-65112CA19BCC}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{A602074D-93F6-4DC7-9C39-65112CA19BCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Kabelleiter - KL 60 (2)" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Kabelleiter - KL 60 (2)'!$A$1:$D$16</definedName>
+    <definedName name="ExternalData_1" localSheetId="0" hidden="1">'Kabelleiter - KL 60 (2)'!$A$1:$D$46</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="56">
   <si>
     <t>Width [mm]</t>
   </si>
@@ -122,6 +122,99 @@
   </si>
   <si>
     <t>WSL 105.600 E3</t>
+  </si>
+  <si>
+    <t>KL 100.203</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>KL 100.303</t>
+  </si>
+  <si>
+    <t>KL 100.403</t>
+  </si>
+  <si>
+    <t>KL 100.503</t>
+  </si>
+  <si>
+    <t>KL 100.603</t>
+  </si>
+  <si>
+    <t>KL 100.203 F</t>
+  </si>
+  <si>
+    <t>KL 100.303 F</t>
+  </si>
+  <si>
+    <t>KL 100.403 F</t>
+  </si>
+  <si>
+    <t>KL 100.503 F</t>
+  </si>
+  <si>
+    <t>KL 100.603 F</t>
+  </si>
+  <si>
+    <t>KL 60.203</t>
+  </si>
+  <si>
+    <t>KL 60.303</t>
+  </si>
+  <si>
+    <t>KL 60.403</t>
+  </si>
+  <si>
+    <t>KL 60.503</t>
+  </si>
+  <si>
+    <t>KL 60.603</t>
+  </si>
+  <si>
+    <t>KL 60.203 F</t>
+  </si>
+  <si>
+    <t>KL 60.303 F</t>
+  </si>
+  <si>
+    <t>KL 60.403 F</t>
+  </si>
+  <si>
+    <t>KL 60.503 F</t>
+  </si>
+  <si>
+    <t>KL 60.603 F</t>
+  </si>
+  <si>
+    <t>KL 60.203 E3</t>
+  </si>
+  <si>
+    <t>KL 60.303 E3</t>
+  </si>
+  <si>
+    <t>KL 60.403 E3</t>
+  </si>
+  <si>
+    <t>KL 60.503 E3</t>
+  </si>
+  <si>
+    <t>KL 60.603 E3</t>
+  </si>
+  <si>
+    <t>KL 60.203 E5</t>
+  </si>
+  <si>
+    <t>KL 60.303 E5</t>
+  </si>
+  <si>
+    <t>KL 60.403 E5</t>
+  </si>
+  <si>
+    <t>KL 60.503 E5</t>
+  </si>
+  <si>
+    <t>KL 60.603 E5</t>
   </si>
 </sst>
 </file>
@@ -141,15 +234,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -157,30 +256,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="164" formatCode="0.0000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0000"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -222,13 +344,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD5A5B1D-E915-4C33-BEF0-B99CEB499BC7}" name="Kabelleiter2829" displayName="Kabelleiter2829" ref="A1:D16" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:D16" xr:uid="{3EA373D9-8131-40C6-9ACA-9C0B9CE0A168}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BD5A5B1D-E915-4C33-BEF0-B99CEB499BC7}" name="Kabelleiter2829" displayName="Kabelleiter2829" ref="A1:D46" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:D46" xr:uid="{3EA373D9-8131-40C6-9ACA-9C0B9CE0A168}"/>
   <tableColumns count="4">
     <tableColumn id="2" xr3:uid="{CA27AB79-E246-494C-82DF-C1A4D65D297D}" uniqueName="2" name="Type" queryTableFieldId="2" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{A3A09EB9-0F46-4979-9B53-E88C55602C55}" uniqueName="3" name="Height [mm]" queryTableFieldId="3" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{1E3D222A-269D-40FE-A0B2-0DC6D0D19682}" uniqueName="4" name="Width [mm]" queryTableFieldId="4" dataDxfId="0"/>
-    <tableColumn id="8" xr3:uid="{1EE0EE5C-58D8-48E4-BDF5-CEE23F601CD8}" uniqueName="8" name="Weight [kg/m]" queryTableFieldId="8" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{1E3D222A-269D-40FE-A0B2-0DC6D0D19682}" uniqueName="4" name="Width [mm]" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{1EE0EE5C-58D8-48E4-BDF5-CEE23F601CD8}" uniqueName="8" name="Weight [kg/m]" queryTableFieldId="8" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -551,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7781E9A-ED86-46FD-BDA6-643C2E22ADF4}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="D27" sqref="D27:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -580,229 +702,634 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="4" t="s">
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="6">
+      <c r="D2" s="3">
         <v>5.4614000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A3" s="4" t="s">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="3">
         <v>5.7336</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A4" s="4" t="s">
+      <c r="A4" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>6.0057999999999998</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A5" s="4" t="s">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="3">
         <v>6.2603999999999997</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A6" s="4" t="s">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="3">
         <v>6.5326000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A7" s="4" t="s">
+      <c r="A7" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="3">
         <v>6.0132000000000003</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A8" s="4" t="s">
+      <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
         <v>5</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="3">
         <v>6.3125999999999998</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="4" t="s">
+      <c r="A9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9" s="4" t="s">
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="3">
         <v>6.6120000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="4" t="s">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="4" t="s">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="3">
         <v>6.8921000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A11" s="4" t="s">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D11" s="3">
         <v>7.1914999999999996</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A12" s="5" t="s">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="6">
+      <c r="D12" s="3">
         <v>5.4962999999999997</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A13" s="5" t="s">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="3">
         <v>5.7702</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A14" s="5" t="s">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="3" t="s">
+      <c r="B14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="3">
         <v>6.0441000000000003</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A15" s="5" t="s">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" s="3" t="s">
+      <c r="B15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="3">
         <v>6.3003999999999998</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A16" s="5" t="s">
+      <c r="A16" t="s">
         <v>24</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="3" t="s">
+      <c r="B16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="6">
+      <c r="D16" s="3">
         <v>6.5743</v>
       </c>
     </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.45">
-      <c r="D21" s="2"/>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="5">
+        <v>3.5091999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6">
+        <v>3.7065000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="5">
+        <v>3.9037999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="6">
+        <v>4.101</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="5">
+        <v>4.2983000000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="6">
+        <v>3.8702000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A23" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5">
+        <v>4.0872000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A24" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="6">
+        <v>4.3041999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A25" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4.5212000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A26" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="7">
+        <v>4.7382</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="2">
+        <v>60</v>
+      </c>
+      <c r="C27" s="2">
+        <v>200</v>
+      </c>
+      <c r="D27" s="9">
+        <v>2.5672000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A28" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="2">
+        <v>60</v>
+      </c>
+      <c r="C28" s="2">
+        <v>300</v>
+      </c>
+      <c r="D28" s="9">
+        <v>2.7645</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A29" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="2">
+        <v>60</v>
+      </c>
+      <c r="C29" s="2">
+        <v>400</v>
+      </c>
+      <c r="D29" s="9">
+        <v>2.9618000000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A30" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B30" s="2">
+        <v>60</v>
+      </c>
+      <c r="C30" s="2">
+        <v>500</v>
+      </c>
+      <c r="D30" s="9">
+        <v>3.1589999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A31" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B31" s="2">
+        <v>60</v>
+      </c>
+      <c r="C31" s="2">
+        <v>600</v>
+      </c>
+      <c r="D31" s="9">
+        <v>3.3563000000000001</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A32" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="2">
+        <v>60</v>
+      </c>
+      <c r="C32" s="2">
+        <v>200</v>
+      </c>
+      <c r="D32" s="9">
+        <v>2.8339999999999899</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A33" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B33" s="2">
+        <v>60</v>
+      </c>
+      <c r="C33" s="2">
+        <v>300</v>
+      </c>
+      <c r="D33" s="9">
+        <v>3.0510000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A34" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="2">
+        <v>60</v>
+      </c>
+      <c r="C34" s="2">
+        <v>400</v>
+      </c>
+      <c r="D34" s="9">
+        <v>3.2679999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A35" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B35" s="2">
+        <v>60</v>
+      </c>
+      <c r="C35" s="2">
+        <v>500</v>
+      </c>
+      <c r="D35" s="9">
+        <v>3.4849999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A36" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" s="2">
+        <v>60</v>
+      </c>
+      <c r="C36" s="2">
+        <v>600</v>
+      </c>
+      <c r="D36" s="9">
+        <v>3.702</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A37" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="2">
+        <v>60</v>
+      </c>
+      <c r="C37" s="2">
+        <v>200</v>
+      </c>
+      <c r="D37" s="9">
+        <v>2.6114999999999999</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A38" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B38" s="2">
+        <v>60</v>
+      </c>
+      <c r="C38" s="2">
+        <v>300</v>
+      </c>
+      <c r="D38" s="9">
+        <v>2.8100999999999998</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A39" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B39" s="2">
+        <v>60</v>
+      </c>
+      <c r="C39" s="2">
+        <v>400</v>
+      </c>
+      <c r="D39" s="9">
+        <v>3.0085999999999999</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A40" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B40" s="2">
+        <v>60</v>
+      </c>
+      <c r="C40" s="2">
+        <v>500</v>
+      </c>
+      <c r="D40" s="9">
+        <v>3.2070999999999898</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A41" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="2">
+        <v>60</v>
+      </c>
+      <c r="C41" s="2">
+        <v>600</v>
+      </c>
+      <c r="D41" s="9">
+        <v>3.4056999999999999</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A42" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B42" s="2">
+        <v>60</v>
+      </c>
+      <c r="C42" s="2">
+        <v>200</v>
+      </c>
+      <c r="D42" s="9">
+        <v>2.6097999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A43" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" s="2">
+        <v>60</v>
+      </c>
+      <c r="C43" s="2">
+        <v>300</v>
+      </c>
+      <c r="D43" s="9">
+        <v>2.8104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A44" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B44" s="2">
+        <v>60</v>
+      </c>
+      <c r="C44" s="2">
+        <v>400</v>
+      </c>
+      <c r="D44" s="9">
+        <v>3.0108999999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A45" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="2">
+        <v>60</v>
+      </c>
+      <c r="C45" s="2">
+        <v>500</v>
+      </c>
+      <c r="D45" s="9">
+        <v>3.2113999999999998</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A46" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B46" s="2">
+        <v>60</v>
+      </c>
+      <c r="C46" s="2">
+        <v>600</v>
+      </c>
+      <c r="D46" s="9">
+        <v>3.4119999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>